<commit_message>
Update Boardgamers em Portugal_BD.xlsx
</commit_message>
<xml_diff>
--- a/Boardgamers em Portugal_BD.xlsx
+++ b/Boardgamers em Portugal_BD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Documents\GitHub\BoardgamingPortugal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC0EA4E0-6AD9-42D9-93A3-612819A6DA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6F0E65-8C06-42AF-8817-C541BA885442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRIADORES DE CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="710">
   <si>
     <t>Criadores de conteudo</t>
   </si>
@@ -1079,9 +1079,6 @@
   </si>
   <si>
     <t>https://open.spotify.com/show/5iJOTNws77TmouVAaX5x97?si=-m0XS1dOR-ag9Vbtna0KNw&amp;utm_source=copy-link</t>
-  </si>
-  <si>
-    <t xml:space="preserve">	⚠️ EM ACTUALIZAÇÃO ⚠️	</t>
   </si>
   <si>
     <t>Nome</t>
@@ -1941,9 +1938,6 @@
     <t>https://maps.app.goo.gl/XpvYdZNTFuxuNqbP8</t>
   </si>
   <si>
-    <t>EDITORAS</t>
-  </si>
-  <si>
     <t>http://www.mebo.pt/</t>
   </si>
   <si>
@@ -1978,15 +1972,6 @@
   </si>
   <si>
     <t>https://www.cardslabgames.com/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REDE BOARDGAME FRIENDLY </t>
-  </si>
-  <si>
-    <t>espaços (cafés, bares, pastelarias e afins) onde se reúnem e ocorrem actividades</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  relacionadas com jogos de tabuleiro modernos (board games)</t>
   </si>
   <si>
     <t>ESPAÇOS</t>
@@ -2304,13 +2289,22 @@
   </si>
   <si>
     <t>18 a 20 de Outubro de 2024</t>
+  </si>
+  <si>
+    <t>Loja</t>
+  </si>
+  <si>
+    <t>Editora</t>
+  </si>
+  <si>
+    <t>Loja/Editora</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="50" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2537,42 +2531,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -2618,18 +2578,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="32">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor theme="8"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2771,18 +2725,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4A86E8"/>
-        <bgColor rgb="FF4A86E8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF6FA8DC"/>
         <bgColor rgb="FF6FA8DC"/>
       </patternFill>
@@ -2806,7 +2748,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -2814,92 +2756,34 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2908,16 +2792,16 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2938,202 +2822,155 @@
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="40" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="37" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="44" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="45" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="46" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="41" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="49" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="16" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3354,7 +3191,7 @@
   </sheetPr>
   <dimension ref="A1:J1045"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
@@ -8402,11 +8239,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H59"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8421,1032 +8258,1017 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="83" t="s">
+      <c r="A1" s="44" t="s">
         <v>341</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
+      <c r="B1" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>343</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>345</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>346</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>347</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>343</v>
-      </c>
-      <c r="C2" s="46" t="s">
-        <v>344</v>
-      </c>
-      <c r="D2" s="46" t="s">
-        <v>345</v>
-      </c>
-      <c r="E2" s="46" t="s">
-        <v>346</v>
-      </c>
-      <c r="F2" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="G2" s="46" t="s">
+      <c r="A2" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="H2" s="46" t="s">
-        <v>8</v>
-      </c>
+      <c r="B2" s="47" t="s">
+        <v>349</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="47" t="s">
-        <v>349</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>350</v>
-      </c>
-      <c r="C3" s="49" t="s">
+      <c r="A3" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
+      <c r="B3" s="47" t="s">
+        <v>352</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>353</v>
+      </c>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="47" t="s">
-        <v>352</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>353</v>
-      </c>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
+      <c r="B4" s="49" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="47" t="s">
-        <v>355</v>
-      </c>
-      <c r="B5" s="50" t="s">
-        <v>356</v>
-      </c>
-      <c r="C5" s="49" t="s">
+      <c r="A5" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
+      <c r="B5" s="49" t="s">
+        <v>358</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>360</v>
+      </c>
+      <c r="E5" s="46"/>
+      <c r="F5" s="49" t="s">
+        <v>361</v>
+      </c>
+      <c r="G5" s="47" t="s">
+        <v>362</v>
+      </c>
+      <c r="H5" s="47" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="47" t="s">
-        <v>358</v>
-      </c>
-      <c r="B6" s="50" t="s">
-        <v>359</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>360</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>361</v>
-      </c>
-      <c r="E6" s="47"/>
-      <c r="F6" s="50" t="s">
-        <v>362</v>
-      </c>
-      <c r="G6" s="48" t="s">
-        <v>363</v>
-      </c>
-      <c r="H6" s="48" t="s">
+      <c r="A6" s="46" t="s">
         <v>364</v>
       </c>
+      <c r="B6" s="47" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>366</v>
+      </c>
+      <c r="D6" s="46"/>
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="47" t="s">
-        <v>365</v>
-      </c>
-      <c r="B7" s="48" t="s">
-        <v>366</v>
-      </c>
-      <c r="C7" s="49" t="s">
+      <c r="A7" s="46" t="s">
         <v>367</v>
       </c>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
+      <c r="B7" s="47" t="s">
+        <v>368</v>
+      </c>
+      <c r="C7" s="48" t="s">
+        <v>369</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="47" t="s">
-        <v>368</v>
-      </c>
-      <c r="B8" s="48" t="s">
-        <v>369</v>
-      </c>
-      <c r="C8" s="49" t="s">
+      <c r="A8" s="46" t="s">
         <v>370</v>
       </c>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
+      <c r="B8" s="47" t="s">
+        <v>371</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>372</v>
+      </c>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="47" t="s">
-        <v>371</v>
-      </c>
-      <c r="B9" s="48" t="s">
+      <c r="A9" s="46" t="s">
+        <v>373</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="C9" s="48" t="s">
+        <v>375</v>
+      </c>
+      <c r="D9" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="46" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>378</v>
+      </c>
+      <c r="C10" s="48" t="s">
+        <v>379</v>
+      </c>
+      <c r="D10" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="46" t="s">
+        <v>381</v>
+      </c>
+      <c r="B11" s="49" t="s">
+        <v>382</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>383</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>384</v>
+      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>385</v>
+      </c>
+      <c r="B12" s="49" t="s">
+        <v>386</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>387</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>388</v>
+      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="49" t="s">
+        <v>389</v>
+      </c>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="46" t="s">
+        <v>390</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>392</v>
+      </c>
+      <c r="D13" s="46"/>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="46" t="s">
+        <v>393</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>394</v>
+      </c>
+      <c r="C14" s="48" t="s">
         <v>372</v>
       </c>
-      <c r="C9" s="49" t="s">
-        <v>373</v>
-      </c>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="47" t="s">
-        <v>374</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>375</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>376</v>
-      </c>
-      <c r="D10" s="47" t="s">
-        <v>377</v>
-      </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="47" t="s">
-        <v>378</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>379</v>
-      </c>
-      <c r="C11" s="49" t="s">
-        <v>380</v>
-      </c>
-      <c r="D11" s="47" t="s">
-        <v>381</v>
-      </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="47"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="47" t="s">
-        <v>382</v>
-      </c>
-      <c r="B12" s="50" t="s">
+      <c r="D14" s="49" t="s">
+        <v>395</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>396</v>
+      </c>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="46" t="s">
+        <v>398</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>399</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>400</v>
+      </c>
+      <c r="D15" s="46"/>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
+        <v>401</v>
+      </c>
+      <c r="B16" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>402</v>
+      </c>
+      <c r="D16" s="46" t="s">
+        <v>403</v>
+      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="47" t="s">
+        <v>404</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="46" t="s">
+        <v>405</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>406</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>407</v>
+      </c>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="46" t="s">
+        <v>408</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>409</v>
+      </c>
+      <c r="C18" s="48" t="s">
+        <v>410</v>
+      </c>
+      <c r="D18" s="46"/>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="46" t="s">
+        <v>411</v>
+      </c>
+      <c r="B19" s="49" t="s">
+        <v>412</v>
+      </c>
+      <c r="C19" s="48" t="s">
+        <v>413</v>
+      </c>
+      <c r="D19" s="46"/>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="46" t="s">
+        <v>414</v>
+      </c>
+      <c r="B20" s="49" t="s">
+        <v>415</v>
+      </c>
+      <c r="C20" s="48" t="s">
+        <v>416</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="46" t="s">
+        <v>417</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>418</v>
+      </c>
+      <c r="C21" s="48" t="s">
+        <v>419</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>420</v>
+      </c>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="46" t="s">
+        <v>421</v>
+      </c>
+      <c r="B22" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>423</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>424</v>
+      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="46" t="s">
+        <v>425</v>
+      </c>
+      <c r="B23" s="51" t="s">
+        <v>426</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>427</v>
+      </c>
+      <c r="D23" s="46"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="46" t="s">
+        <v>428</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>429</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>430</v>
+      </c>
+      <c r="D24" s="46"/>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="46" t="s">
+        <v>431</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>432</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>402</v>
+      </c>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="46" t="s">
+        <v>433</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>434</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>435</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>437</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="46" t="s">
+        <v>439</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>440</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>441</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>442</v>
+      </c>
+      <c r="E28" s="46"/>
+      <c r="F28" s="47" t="s">
+        <v>404</v>
+      </c>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>444</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>387</v>
+      </c>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="46" t="s">
+        <v>445</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>446</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>447</v>
+      </c>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>449</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>450</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>451</v>
+      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="46" t="s">
+        <v>452</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>453</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>454</v>
+      </c>
+      <c r="D32" s="46"/>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>456</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>457</v>
+      </c>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="46" t="s">
+        <v>458</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>459</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>460</v>
+      </c>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="46" t="s">
+        <v>461</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>462</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>463</v>
+      </c>
+      <c r="D35" s="46" t="s">
+        <v>464</v>
+      </c>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="46" t="s">
+        <v>465</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>466</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>467</v>
+      </c>
+      <c r="D36" s="46"/>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="46" t="s">
+        <v>468</v>
+      </c>
+      <c r="B37" s="49" t="s">
+        <v>469</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="D37" s="46" t="s">
+        <v>471</v>
+      </c>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="46" t="s">
+        <v>472</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>473</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="D38" s="46"/>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="46" t="s">
+        <v>475</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>476</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="D39" s="46"/>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="46" t="s">
+        <v>477</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>252</v>
+      </c>
+      <c r="C40" s="48" t="s">
         <v>383</v>
       </c>
-      <c r="C12" s="49" t="s">
-        <v>384</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>385</v>
-      </c>
-      <c r="E12" s="47"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="47"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="47" t="s">
-        <v>386</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>387</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>388</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>389</v>
-      </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="50" t="s">
-        <v>390</v>
-      </c>
-      <c r="G13" s="47"/>
-      <c r="H13" s="47"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="47" t="s">
-        <v>391</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>392</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>393</v>
-      </c>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="47" t="s">
-        <v>394</v>
-      </c>
-      <c r="B15" s="48" t="s">
-        <v>395</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>373</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>396</v>
-      </c>
-      <c r="E15" s="48" t="s">
-        <v>397</v>
-      </c>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="48" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="47" t="s">
-        <v>399</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>400</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>401</v>
-      </c>
-      <c r="D16" s="47"/>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="47" t="s">
-        <v>402</v>
-      </c>
-      <c r="B17" s="50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C17" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="D17" s="47" t="s">
-        <v>404</v>
-      </c>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48" t="s">
-        <v>405</v>
-      </c>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="47" t="s">
-        <v>406</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>407</v>
-      </c>
-      <c r="C18" s="49" t="s">
-        <v>408</v>
-      </c>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="47" t="s">
-        <v>409</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>410</v>
-      </c>
-      <c r="C19" s="49" t="s">
-        <v>411</v>
-      </c>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="47" t="s">
-        <v>412</v>
-      </c>
-      <c r="B20" s="50" t="s">
+      <c r="D40" s="46" t="s">
+        <v>478</v>
+      </c>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>259</v>
+      </c>
+      <c r="C41" s="48" t="s">
         <v>413</v>
       </c>
-      <c r="C20" s="49" t="s">
-        <v>414</v>
-      </c>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="47" t="s">
-        <v>415</v>
-      </c>
-      <c r="B21" s="50" t="s">
-        <v>416</v>
-      </c>
-      <c r="C21" s="49" t="s">
-        <v>417</v>
-      </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="47" t="s">
-        <v>418</v>
-      </c>
-      <c r="B22" s="48" t="s">
-        <v>419</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>420</v>
-      </c>
-      <c r="D22" s="47" t="s">
-        <v>421</v>
-      </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="47" t="s">
-        <v>422</v>
-      </c>
-      <c r="B23" s="51" t="s">
-        <v>423</v>
-      </c>
-      <c r="C23" s="49" t="s">
-        <v>424</v>
-      </c>
-      <c r="D23" s="50" t="s">
-        <v>425</v>
-      </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="47" t="s">
-        <v>426</v>
-      </c>
-      <c r="B24" s="52" t="s">
-        <v>427</v>
-      </c>
-      <c r="C24" s="49" t="s">
-        <v>428</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="47" t="s">
-        <v>429</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>430</v>
-      </c>
-      <c r="C25" s="49" t="s">
-        <v>431</v>
-      </c>
-      <c r="D25" s="47"/>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="47" t="s">
-        <v>432</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>433</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>403</v>
-      </c>
-      <c r="D26" s="47"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="47" t="s">
-        <v>434</v>
-      </c>
-      <c r="B27" s="48" t="s">
-        <v>435</v>
-      </c>
-      <c r="C27" s="49" t="s">
-        <v>436</v>
-      </c>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="47"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="47" t="s">
-        <v>437</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>438</v>
-      </c>
-      <c r="C28" s="49" t="s">
-        <v>439</v>
-      </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="47"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="47" t="s">
-        <v>440</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>441</v>
-      </c>
-      <c r="C29" s="49" t="s">
-        <v>442</v>
-      </c>
-      <c r="D29" s="47" t="s">
-        <v>443</v>
-      </c>
-      <c r="E29" s="47"/>
-      <c r="F29" s="48" t="s">
-        <v>405</v>
-      </c>
-      <c r="G29" s="47"/>
-      <c r="H29" s="47"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="47" t="s">
-        <v>444</v>
-      </c>
-      <c r="B30" s="48" t="s">
-        <v>445</v>
-      </c>
-      <c r="C30" s="49" t="s">
-        <v>388</v>
-      </c>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="47" t="s">
-        <v>446</v>
-      </c>
-      <c r="B31" s="48" t="s">
-        <v>447</v>
-      </c>
-      <c r="C31" s="49" t="s">
-        <v>448</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="47" t="s">
-        <v>449</v>
-      </c>
-      <c r="B32" s="48" t="s">
-        <v>450</v>
-      </c>
-      <c r="C32" s="49" t="s">
-        <v>451</v>
-      </c>
-      <c r="D32" s="50" t="s">
-        <v>452</v>
-      </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="47" t="s">
-        <v>453</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>454</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>455</v>
-      </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="47"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="47" t="s">
-        <v>456</v>
-      </c>
-      <c r="B34" s="48" t="s">
-        <v>457</v>
-      </c>
-      <c r="C34" s="49" t="s">
-        <v>458</v>
-      </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="47" t="s">
-        <v>459</v>
-      </c>
-      <c r="B35" s="48" t="s">
-        <v>460</v>
-      </c>
-      <c r="C35" s="49" t="s">
-        <v>461</v>
-      </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="47"/>
-      <c r="G35" s="47"/>
-      <c r="H35" s="47"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="47" t="s">
-        <v>462</v>
-      </c>
-      <c r="B36" s="48" t="s">
-        <v>463</v>
-      </c>
-      <c r="C36" s="49" t="s">
-        <v>464</v>
-      </c>
-      <c r="D36" s="47" t="s">
-        <v>465</v>
-      </c>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="47" t="s">
-        <v>466</v>
-      </c>
-      <c r="B37" s="48" t="s">
-        <v>467</v>
-      </c>
-      <c r="C37" s="49" t="s">
-        <v>468</v>
-      </c>
-      <c r="D37" s="47"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="47"/>
-      <c r="H37" s="47"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="47" t="s">
-        <v>469</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>470</v>
-      </c>
-      <c r="C38" s="49" t="s">
-        <v>471</v>
-      </c>
-      <c r="D38" s="47" t="s">
-        <v>472</v>
-      </c>
-      <c r="E38" s="47"/>
-      <c r="F38" s="47"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="47"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="47" t="s">
-        <v>473</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>474</v>
-      </c>
-      <c r="C39" s="49" t="s">
-        <v>475</v>
-      </c>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="47" t="s">
-        <v>476</v>
-      </c>
-      <c r="B40" s="48" t="s">
-        <v>477</v>
-      </c>
-      <c r="C40" s="49" t="s">
-        <v>471</v>
-      </c>
-      <c r="D40" s="47"/>
-      <c r="E40" s="47"/>
-      <c r="F40" s="47"/>
-      <c r="G40" s="47"/>
-      <c r="H40" s="47"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="47" t="s">
-        <v>478</v>
-      </c>
-      <c r="B41" s="48" t="s">
-        <v>252</v>
-      </c>
-      <c r="C41" s="49" t="s">
-        <v>384</v>
-      </c>
-      <c r="D41" s="47" t="s">
+      <c r="D41" s="46"/>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="46" t="s">
         <v>479</v>
       </c>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="47" t="s">
-        <v>257</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>259</v>
-      </c>
-      <c r="C42" s="49" t="s">
-        <v>414</v>
-      </c>
-      <c r="D42" s="47"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="47"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="47"/>
+      <c r="B42" s="47" t="s">
+        <v>480</v>
+      </c>
+      <c r="C42" s="48" t="s">
+        <v>481</v>
+      </c>
+      <c r="D42" s="46"/>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="47" t="s">
-        <v>480</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>481</v>
-      </c>
-      <c r="C43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>482</v>
       </c>
-      <c r="D43" s="47"/>
-      <c r="E43" s="47"/>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
-      <c r="H43" s="47"/>
+      <c r="B43" s="47" t="s">
+        <v>483</v>
+      </c>
+      <c r="C43" s="48" t="s">
+        <v>484</v>
+      </c>
+      <c r="D43" s="46"/>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="47" t="s">
-        <v>483</v>
-      </c>
-      <c r="B44" s="48" t="s">
-        <v>484</v>
-      </c>
-      <c r="C44" s="49" t="s">
+      <c r="A44" s="52"/>
+      <c r="B44" s="52" t="s">
         <v>485</v>
       </c>
-      <c r="D44" s="47"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="47"/>
-      <c r="H44" s="47"/>
+      <c r="C44" s="53"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53" t="s">
+      <c r="A45" s="46" t="s">
         <v>486</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="53"/>
-      <c r="G45" s="53"/>
-      <c r="H45" s="53"/>
+      <c r="B45" s="47" t="s">
+        <v>487</v>
+      </c>
+      <c r="C45" s="48"/>
+      <c r="D45" s="46"/>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="47" t="s">
-        <v>487</v>
-      </c>
-      <c r="B46" s="48" t="s">
+      <c r="A46" s="46" t="s">
         <v>488</v>
       </c>
-      <c r="C46" s="49"/>
-      <c r="D46" s="47"/>
-      <c r="E46" s="47"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="47"/>
-      <c r="H46" s="47"/>
+      <c r="B46" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="C46" s="48"/>
+      <c r="D46" s="46"/>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="47" t="s">
-        <v>489</v>
-      </c>
-      <c r="B47" s="48" t="s">
+      <c r="A47" s="46" t="s">
         <v>490</v>
       </c>
-      <c r="C47" s="49"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
+      <c r="B47" s="47" t="s">
+        <v>491</v>
+      </c>
+      <c r="C47" s="48" t="s">
+        <v>383</v>
+      </c>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="47" t="s">
-        <v>491</v>
-      </c>
-      <c r="B48" s="48" t="s">
+      <c r="A48" s="46" t="s">
         <v>492</v>
       </c>
-      <c r="C48" s="49" t="s">
-        <v>384</v>
-      </c>
-      <c r="D48" s="47"/>
-      <c r="E48" s="47"/>
-      <c r="F48" s="47"/>
-      <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
+      <c r="B48" s="47" t="s">
+        <v>493</v>
+      </c>
+      <c r="C48" s="48"/>
+      <c r="D48" s="46"/>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="47" t="s">
-        <v>493</v>
-      </c>
-      <c r="B49" s="48" t="s">
+      <c r="A49" s="46" t="s">
         <v>494</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="47"/>
-      <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="47"/>
+      <c r="B49" s="47" t="s">
+        <v>495</v>
+      </c>
+      <c r="C49" s="48"/>
+      <c r="D49" s="46"/>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="47" t="s">
-        <v>495</v>
-      </c>
-      <c r="B50" s="48" t="s">
+      <c r="A50" s="46" t="s">
         <v>496</v>
       </c>
-      <c r="C50" s="49"/>
-      <c r="D50" s="47"/>
-      <c r="E50" s="47"/>
-      <c r="F50" s="47"/>
-      <c r="G50" s="47"/>
-      <c r="H50" s="47"/>
+      <c r="B50" s="47" t="s">
+        <v>497</v>
+      </c>
+      <c r="C50" s="48"/>
+      <c r="D50" s="46"/>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="47" t="s">
-        <v>497</v>
-      </c>
-      <c r="B51" s="48" t="s">
+      <c r="A51" s="46" t="s">
         <v>498</v>
       </c>
-      <c r="C51" s="49"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="47"/>
-      <c r="H51" s="47"/>
+      <c r="B51" s="47" t="s">
+        <v>499</v>
+      </c>
+      <c r="C51" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="47" t="s">
-        <v>499</v>
-      </c>
-      <c r="B52" s="48" t="s">
-        <v>500</v>
-      </c>
-      <c r="C52" s="49" t="s">
+      <c r="A52" s="46" t="s">
         <v>501</v>
       </c>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
-      <c r="F52" s="47"/>
-      <c r="G52" s="47"/>
-      <c r="H52" s="47"/>
+      <c r="B52" s="47" t="s">
+        <v>502</v>
+      </c>
+      <c r="C52" s="48"/>
+      <c r="D52" s="46"/>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="47" t="s">
-        <v>502</v>
-      </c>
-      <c r="B53" s="48" t="s">
+      <c r="A53" s="46" t="s">
         <v>503</v>
       </c>
-      <c r="C53" s="49"/>
-      <c r="D53" s="47"/>
-      <c r="E53" s="47"/>
-      <c r="F53" s="47"/>
-      <c r="G53" s="47"/>
-      <c r="H53" s="47"/>
+      <c r="B53" s="47" t="s">
+        <v>504</v>
+      </c>
+      <c r="C53" s="48"/>
+      <c r="D53" s="46"/>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="47" t="s">
-        <v>504</v>
-      </c>
-      <c r="B54" s="48" t="s">
+      <c r="A54" s="46" t="s">
         <v>505</v>
       </c>
-      <c r="C54" s="49"/>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
-      <c r="F54" s="47"/>
-      <c r="G54" s="47"/>
-      <c r="H54" s="47"/>
+      <c r="B54" s="49" t="s">
+        <v>506</v>
+      </c>
+      <c r="C54" s="48" t="s">
+        <v>507</v>
+      </c>
+      <c r="D54" s="46"/>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="47" t="s">
-        <v>506</v>
-      </c>
-      <c r="B55" s="50" t="s">
-        <v>507</v>
-      </c>
-      <c r="C55" s="49" t="s">
+      <c r="A55" s="53"/>
+      <c r="B55" s="53" t="s">
         <v>508</v>
       </c>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="47"/>
-      <c r="H55" s="47"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="52"/>
+      <c r="G55" s="52"/>
+      <c r="H55" s="52"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="54"/>
-      <c r="B56" s="54" t="s">
+      <c r="A56" s="46" t="s">
         <v>509</v>
       </c>
-      <c r="C56" s="54"/>
-      <c r="D56" s="53"/>
-      <c r="E56" s="53"/>
-      <c r="F56" s="53"/>
-      <c r="G56" s="53"/>
-      <c r="H56" s="53"/>
+      <c r="B56" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="C56" s="48"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="47" t="s">
-        <v>510</v>
-      </c>
-      <c r="B57" s="48" t="s">
+      <c r="A57" s="46" t="s">
         <v>511</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="47"/>
-      <c r="E57" s="47"/>
-      <c r="F57" s="47"/>
-      <c r="G57" s="47"/>
-      <c r="H57" s="47"/>
+      <c r="B57" s="47" t="s">
+        <v>512</v>
+      </c>
+      <c r="C57" s="48"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="47" t="s">
-        <v>512</v>
-      </c>
-      <c r="B58" s="48" t="s">
-        <v>513</v>
-      </c>
-      <c r="C58" s="49"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
-      <c r="H58" s="47"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C59" s="55"/>
+      <c r="C58" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:H1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B5" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="B6" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
-    <hyperlink ref="F6" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
-    <hyperlink ref="G6" r:id="rId7" location="CjQKIObolfr3kjhoqpaahhROvCk0XzgpqdEh6-hojizTnIN_EhA4IMJR3TVtNd9qIb1lYPin" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
-    <hyperlink ref="H6" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
-    <hyperlink ref="B8" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
-    <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
-    <hyperlink ref="B10" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
-    <hyperlink ref="B11" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="B12" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D12" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="B13" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="F13" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="B14" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="B15" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="D15" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
-    <hyperlink ref="E15" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
-    <hyperlink ref="H15" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
-    <hyperlink ref="B16" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
-    <hyperlink ref="B17" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
-    <hyperlink ref="F17" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
-    <hyperlink ref="B18" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
-    <hyperlink ref="B19" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
-    <hyperlink ref="B20" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
-    <hyperlink ref="B21" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
-    <hyperlink ref="B22" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
-    <hyperlink ref="B23" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
-    <hyperlink ref="D23" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
-    <hyperlink ref="B24" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
-    <hyperlink ref="B25" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
-    <hyperlink ref="B26" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
-    <hyperlink ref="B27" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
-    <hyperlink ref="B28" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
-    <hyperlink ref="B29" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
-    <hyperlink ref="F29" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
-    <hyperlink ref="B30" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
-    <hyperlink ref="B31" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
-    <hyperlink ref="B32" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
-    <hyperlink ref="D32" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
-    <hyperlink ref="B33" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
-    <hyperlink ref="B34" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
-    <hyperlink ref="B35" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
-    <hyperlink ref="B36" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
-    <hyperlink ref="B37" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
-    <hyperlink ref="B38" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
-    <hyperlink ref="B39" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
-    <hyperlink ref="B40" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
-    <hyperlink ref="B41" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
-    <hyperlink ref="B42" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
-    <hyperlink ref="B43" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
-    <hyperlink ref="B44" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
-    <hyperlink ref="B46" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
-    <hyperlink ref="B47" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
-    <hyperlink ref="B48" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
-    <hyperlink ref="B49" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
-    <hyperlink ref="B50" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
-    <hyperlink ref="B51" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
-    <hyperlink ref="B52" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
-    <hyperlink ref="B53" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
-    <hyperlink ref="B54" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
-    <hyperlink ref="B55" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
-    <hyperlink ref="B57" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
-    <hyperlink ref="B58" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="G5" r:id="rId7" location="CjQKIObolfr3kjhoqpaahhROvCk0XzgpqdEh6-hojizTnIN_EhA4IMJR3TVtNd9qIb1lYPin" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="H5" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B6" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B7" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="B9" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B10" r:id="rId13" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="D11" r:id="rId15" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="B12" r:id="rId16" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="F12" r:id="rId17" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="B13" r:id="rId18" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="B14" r:id="rId19" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="D14" r:id="rId20" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="E14" r:id="rId21" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="H14" r:id="rId22" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="B15" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="B16" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="F16" r:id="rId25" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="B17" r:id="rId26" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="B18" r:id="rId27" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="B19" r:id="rId28" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="B20" r:id="rId29" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="B21" r:id="rId30" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
+    <hyperlink ref="B22" r:id="rId31" xr:uid="{00000000-0004-0000-0100-00001E000000}"/>
+    <hyperlink ref="D22" r:id="rId32" xr:uid="{00000000-0004-0000-0100-00001F000000}"/>
+    <hyperlink ref="B23" r:id="rId33" xr:uid="{00000000-0004-0000-0100-000020000000}"/>
+    <hyperlink ref="B24" r:id="rId34" xr:uid="{00000000-0004-0000-0100-000021000000}"/>
+    <hyperlink ref="B25" r:id="rId35" xr:uid="{00000000-0004-0000-0100-000022000000}"/>
+    <hyperlink ref="B26" r:id="rId36" xr:uid="{00000000-0004-0000-0100-000023000000}"/>
+    <hyperlink ref="B27" r:id="rId37" xr:uid="{00000000-0004-0000-0100-000024000000}"/>
+    <hyperlink ref="B28" r:id="rId38" xr:uid="{00000000-0004-0000-0100-000025000000}"/>
+    <hyperlink ref="F28" r:id="rId39" xr:uid="{00000000-0004-0000-0100-000026000000}"/>
+    <hyperlink ref="B29" r:id="rId40" xr:uid="{00000000-0004-0000-0100-000027000000}"/>
+    <hyperlink ref="B30" r:id="rId41" xr:uid="{00000000-0004-0000-0100-000028000000}"/>
+    <hyperlink ref="B31" r:id="rId42" xr:uid="{00000000-0004-0000-0100-000029000000}"/>
+    <hyperlink ref="D31" r:id="rId43" xr:uid="{00000000-0004-0000-0100-00002A000000}"/>
+    <hyperlink ref="B32" r:id="rId44" xr:uid="{00000000-0004-0000-0100-00002B000000}"/>
+    <hyperlink ref="B33" r:id="rId45" xr:uid="{00000000-0004-0000-0100-00002C000000}"/>
+    <hyperlink ref="B34" r:id="rId46" xr:uid="{00000000-0004-0000-0100-00002D000000}"/>
+    <hyperlink ref="B35" r:id="rId47" xr:uid="{00000000-0004-0000-0100-00002E000000}"/>
+    <hyperlink ref="B36" r:id="rId48" xr:uid="{00000000-0004-0000-0100-00002F000000}"/>
+    <hyperlink ref="B37" r:id="rId49" xr:uid="{00000000-0004-0000-0100-000030000000}"/>
+    <hyperlink ref="B38" r:id="rId50" xr:uid="{00000000-0004-0000-0100-000031000000}"/>
+    <hyperlink ref="B39" r:id="rId51" xr:uid="{00000000-0004-0000-0100-000032000000}"/>
+    <hyperlink ref="B40" r:id="rId52" xr:uid="{00000000-0004-0000-0100-000033000000}"/>
+    <hyperlink ref="B41" r:id="rId53" xr:uid="{00000000-0004-0000-0100-000034000000}"/>
+    <hyperlink ref="B42" r:id="rId54" xr:uid="{00000000-0004-0000-0100-000035000000}"/>
+    <hyperlink ref="B43" r:id="rId55" xr:uid="{00000000-0004-0000-0100-000036000000}"/>
+    <hyperlink ref="B45" r:id="rId56" xr:uid="{00000000-0004-0000-0100-000037000000}"/>
+    <hyperlink ref="B46" r:id="rId57" xr:uid="{00000000-0004-0000-0100-000038000000}"/>
+    <hyperlink ref="B47" r:id="rId58" xr:uid="{00000000-0004-0000-0100-000039000000}"/>
+    <hyperlink ref="B48" r:id="rId59" xr:uid="{00000000-0004-0000-0100-00003A000000}"/>
+    <hyperlink ref="B49" r:id="rId60" xr:uid="{00000000-0004-0000-0100-00003B000000}"/>
+    <hyperlink ref="B50" r:id="rId61" xr:uid="{00000000-0004-0000-0100-00003C000000}"/>
+    <hyperlink ref="B51" r:id="rId62" xr:uid="{00000000-0004-0000-0100-00003D000000}"/>
+    <hyperlink ref="B52" r:id="rId63" xr:uid="{00000000-0004-0000-0100-00003E000000}"/>
+    <hyperlink ref="B53" r:id="rId64" xr:uid="{00000000-0004-0000-0100-00003F000000}"/>
+    <hyperlink ref="B54" r:id="rId65" xr:uid="{00000000-0004-0000-0100-000040000000}"/>
+    <hyperlink ref="B56" r:id="rId66" xr:uid="{00000000-0004-0000-0100-000041000000}"/>
+    <hyperlink ref="B57" r:id="rId67" xr:uid="{00000000-0004-0000-0100-000042000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9457,418 +9279,512 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
-        <v>341</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="55" t="s">
+        <v>513</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>514</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>515</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>515</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
         <v>517</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="C2" s="57" t="s">
         <v>518</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="D2" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="56" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
+      <c r="B3" s="56" t="s">
         <v>520</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="C3" s="57" t="s">
         <v>521</v>
       </c>
-      <c r="C4" s="58" t="s">
+      <c r="D3" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="56" t="s">
+        <v>600</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>601</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="56" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
+      <c r="B5" s="56" t="s">
         <v>523</v>
       </c>
-      <c r="B5" s="57" t="s">
+      <c r="C5" s="57" t="s">
         <v>524</v>
       </c>
-      <c r="C5" s="58" t="s">
+      <c r="D5" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="56" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="57" t="s">
+      <c r="B6" s="56" t="s">
         <v>526</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="C6" s="57" t="s">
         <v>527</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="D6" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="56" t="s">
+        <v>597</v>
+      </c>
+      <c r="B7" s="56" t="s">
+        <v>598</v>
+      </c>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="56" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="57" t="s">
+      <c r="B8" s="56" t="s">
         <v>529</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="C8" s="57" t="s">
         <v>530</v>
       </c>
-      <c r="C7" s="58" t="s">
+      <c r="D8" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="56" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+      <c r="B9" s="56" t="s">
         <v>532</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="C9" s="57" t="s">
         <v>533</v>
       </c>
-      <c r="C8" s="58" t="s">
+      <c r="D9" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>602</v>
+      </c>
+      <c r="B10" s="56" t="s">
+        <v>603</v>
+      </c>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="56" t="s">
+        <v>593</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>594</v>
+      </c>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="56" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>535</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="C12" s="57" t="s">
         <v>536</v>
       </c>
-      <c r="C9" s="58" t="s">
+      <c r="D12" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="56" t="s">
+        <v>534</v>
+      </c>
+      <c r="B13" s="56" t="s">
+        <v>535</v>
+      </c>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="56" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="B14" s="56" t="s">
         <v>538</v>
       </c>
-      <c r="B10" s="57" t="s">
+      <c r="C14" s="57" t="s">
         <v>539</v>
       </c>
-      <c r="C10" s="58" t="s">
+      <c r="D14" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="56" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="B15" s="56" t="s">
         <v>541</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="C15" s="57" t="s">
         <v>542</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="D15" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="56" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="57" t="s">
+      <c r="B16" s="56" t="s">
         <v>544</v>
       </c>
-      <c r="B12" s="57" t="s">
+      <c r="C16" s="57" t="s">
         <v>545</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="D16" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="56" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="57" t="s">
+      <c r="B17" s="56" t="s">
         <v>547</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="C17" s="57" t="s">
         <v>548</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="D17" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="56" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="57" t="s">
+      <c r="B18" s="56" t="s">
         <v>550</v>
       </c>
-      <c r="B14" s="57" t="s">
+      <c r="C18" s="57" t="s">
         <v>551</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="D18" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="56" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="57" t="s">
+      <c r="B19" s="56" t="s">
         <v>553</v>
       </c>
-      <c r="B15" s="57" t="s">
+      <c r="C19" s="57" t="s">
         <v>554</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="D19" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="56" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="57" t="s">
+      <c r="B20" s="56" t="s">
         <v>556</v>
       </c>
-      <c r="B16" s="57" t="s">
+      <c r="C20" s="57" t="s">
         <v>557</v>
       </c>
-      <c r="C16" s="58" t="s">
+      <c r="D20" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="56" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="57" t="s">
+      <c r="B21" s="56" t="s">
         <v>559</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="C21" s="57" t="s">
         <v>560</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="D21" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="56" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="57" t="s">
+      <c r="B22" s="56" t="s">
         <v>562</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="C22" s="57" t="s">
         <v>563</v>
       </c>
-      <c r="C18" s="58" t="s">
+      <c r="D22" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="B23" s="56" t="s">
+        <v>592</v>
+      </c>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="56" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="57" t="s">
+      <c r="B24" s="56" t="s">
         <v>565</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="C24" s="57" t="s">
         <v>566</v>
       </c>
-      <c r="C19" s="58" t="s">
+      <c r="D24" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="56" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="57" t="s">
+      <c r="B25" s="56" t="s">
         <v>568</v>
       </c>
-      <c r="B20" s="57" t="s">
+      <c r="C25" s="57" t="s">
         <v>569</v>
       </c>
-      <c r="C20" s="58" t="s">
+      <c r="D25" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="56" t="s">
+        <v>595</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>596</v>
+      </c>
+      <c r="C26" s="56"/>
+      <c r="D26" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="56" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="57" t="s">
+      <c r="B27" s="56" t="s">
         <v>571</v>
       </c>
-      <c r="B21" s="57" t="s">
+      <c r="C27" s="57" t="s">
         <v>572</v>
       </c>
-      <c r="C21" s="58" t="s">
+      <c r="D27" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="56" t="s">
+        <v>570</v>
+      </c>
+      <c r="B28" s="56" t="s">
+        <v>571</v>
+      </c>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="56" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="57" t="s">
+      <c r="B29" s="56" t="s">
         <v>574</v>
       </c>
-      <c r="B22" s="57" t="s">
+      <c r="C29" s="57" t="s">
         <v>575</v>
       </c>
-      <c r="C22" s="58" t="s">
+      <c r="D29" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="56" t="s">
         <v>576</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="57" t="s">
+      <c r="B30" s="56" t="s">
         <v>577</v>
       </c>
-      <c r="B23" s="57" t="s">
+      <c r="C30" s="57"/>
+      <c r="D30" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="56" t="s">
         <v>578</v>
       </c>
-      <c r="C23" s="58"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="57" t="s">
+      <c r="B31" s="56" t="s">
         <v>579</v>
       </c>
-      <c r="B24" s="57" t="s">
+      <c r="C31" s="57" t="s">
         <v>580</v>
       </c>
-      <c r="C24" s="58" t="s">
+      <c r="D31" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="56" t="s">
         <v>581</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="57" t="s">
+      <c r="B32" s="56" t="s">
         <v>582</v>
       </c>
-      <c r="B25" s="57" t="s">
+      <c r="C32" s="57" t="s">
         <v>583</v>
       </c>
-      <c r="C25" s="58" t="s">
+      <c r="D32" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="56" t="s">
         <v>584</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="57" t="s">
+      <c r="B33" s="56" t="s">
         <v>585</v>
       </c>
-      <c r="B26" s="57" t="s">
+      <c r="C33" s="57" t="s">
         <v>586</v>
       </c>
-      <c r="C26" s="58" t="s">
+      <c r="D33" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="56" t="s">
         <v>587</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="57" t="s">
+      <c r="B34" s="56" t="s">
         <v>588</v>
       </c>
-      <c r="B27" s="57" t="s">
+      <c r="C34" s="57" t="s">
         <v>589</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="D34" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="56" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="57" t="s">
+      <c r="B35" s="56" t="s">
+        <v>588</v>
+      </c>
+      <c r="C35" s="57" t="s">
         <v>591</v>
       </c>
-      <c r="B28" s="57" t="s">
-        <v>589</v>
-      </c>
-      <c r="C28" s="58" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="59" t="s">
-        <v>593</v>
-      </c>
-      <c r="B32" s="59" t="s">
-        <v>515</v>
-      </c>
-      <c r="C32" s="60"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="61" t="s">
-        <v>535</v>
-      </c>
-      <c r="B33" s="61" t="s">
-        <v>536</v>
-      </c>
-      <c r="C33" s="60"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="62" t="s">
-        <v>185</v>
-      </c>
-      <c r="B34" s="62" t="s">
-        <v>594</v>
-      </c>
-      <c r="C34" s="60"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="62" t="s">
-        <v>595</v>
-      </c>
-      <c r="B35" s="62" t="s">
-        <v>596</v>
-      </c>
-      <c r="C35" s="60"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="62" t="s">
-        <v>597</v>
-      </c>
-      <c r="B36" s="62" t="s">
-        <v>598</v>
-      </c>
-      <c r="C36" s="60"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="62" t="s">
+      <c r="D35" s="56" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="56" t="s">
         <v>599</v>
       </c>
-      <c r="B37" s="63" t="s">
-        <v>600</v>
-      </c>
-      <c r="C37" s="64"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="62" t="s">
-        <v>601</v>
-      </c>
-      <c r="B38" s="62" t="s">
+      <c r="B36" s="56" t="s">
         <v>332</v>
       </c>
-      <c r="C38" s="60"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="62" t="s">
-        <v>602</v>
-      </c>
-      <c r="B39" s="62" t="s">
-        <v>603</v>
-      </c>
-      <c r="C39" s="65"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="66" t="s">
-        <v>604</v>
-      </c>
-      <c r="B40" s="66" t="s">
-        <v>605</v>
-      </c>
-      <c r="C40" s="65"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="66" t="s">
-        <v>571</v>
-      </c>
-      <c r="B41" s="57" t="s">
-        <v>572</v>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56" t="s">
+        <v>708</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="A3:C24 A32:B41 C32:C37">
-    <cfRule type="colorScale" priority="1">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D36">
+    <sortCondition ref="A2:A36"/>
+  </sortState>
+  <conditionalFormatting sqref="A2:C23">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -9878,66 +9794,66 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
     <hyperlink ref="B5" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
     <hyperlink ref="C5" r:id="rId6" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
     <hyperlink ref="B6" r:id="rId7" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
     <hyperlink ref="C6" r:id="rId8" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="B7" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="C7" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="B8" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="C8" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="B9" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="C9" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="B10" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="C10" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="B11" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="C11" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="B12" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="C12" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="B13" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="C13" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="B14" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="C14" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="B15" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="C15" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="B16" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="C16" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="B17" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="C17" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="B18" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="C18" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink ref="B19" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink ref="C19" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink ref="B20" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink ref="C20" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink ref="B21" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink ref="C21" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink ref="B22" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink ref="C22" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink ref="B23" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink ref="B24" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink ref="C24" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink ref="B25" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink ref="C25" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink ref="B26" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink ref="C26" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink ref="B27" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink ref="C27" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink ref="B28" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink ref="C28" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
-    <hyperlink ref="B33" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
-    <hyperlink ref="B34" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
-    <hyperlink ref="B35" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
-    <hyperlink ref="B36" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
-    <hyperlink ref="B37" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
-    <hyperlink ref="B38" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
-    <hyperlink ref="B39" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
-    <hyperlink ref="B40" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
-    <hyperlink ref="B41" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="B8" r:id="rId9" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="C8" r:id="rId10" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="C9" r:id="rId12" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B12" r:id="rId13" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="C12" r:id="rId14" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B14" r:id="rId15" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="C14" r:id="rId16" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B15" r:id="rId17" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="C15" r:id="rId18" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="B16" r:id="rId19" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="C16" r:id="rId20" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="B17" r:id="rId21" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="C17" r:id="rId22" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="B18" r:id="rId23" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="C18" r:id="rId24" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="B19" r:id="rId25" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="C19" r:id="rId26" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="B20" r:id="rId27" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="C20" r:id="rId28" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="B21" r:id="rId29" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="C21" r:id="rId30" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="B22" r:id="rId31" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="C22" r:id="rId32" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="B24" r:id="rId33" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="C24" r:id="rId34" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="B25" r:id="rId35" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="C25" r:id="rId36" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="B27" r:id="rId37" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="C27" r:id="rId38" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="B29" r:id="rId39" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="C29" r:id="rId40" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="B30" r:id="rId41" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="B31" r:id="rId42" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="C31" r:id="rId43" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="B32" r:id="rId44" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="C32" r:id="rId45" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="B33" r:id="rId46" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="C33" r:id="rId47" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="B34" r:id="rId48" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="C34" r:id="rId49" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="B35" r:id="rId50" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="C35" r:id="rId51" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="B13" r:id="rId52" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="B23" r:id="rId53" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="B11" r:id="rId54" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="B26" r:id="rId55" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="B7" r:id="rId56" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="B36" r:id="rId57" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="B4" r:id="rId58" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="B10" r:id="rId59" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="B28" r:id="rId60" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9948,11 +9864,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9963,317 +9879,279 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="81" t="s">
-        <v>341</v>
-      </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="67"/>
+      <c r="A1" s="59" t="s">
+        <v>604</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>343</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>605</v>
+      </c>
+      <c r="D1" s="58"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="60" t="s">
         <v>606</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="67"/>
+      <c r="B2" s="60" t="s">
+        <v>407</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>607</v>
+      </c>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="87" t="s">
-        <v>607</v>
-      </c>
-      <c r="B3" s="82"/>
-      <c r="C3" s="82"/>
-      <c r="D3" s="67"/>
+      <c r="A3" s="62" t="s">
+        <v>608</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>402</v>
+      </c>
+      <c r="C3" s="64" t="s">
+        <v>609</v>
+      </c>
+      <c r="D3" s="58"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="88" t="s">
-        <v>608</v>
-      </c>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="67"/>
+      <c r="A4" s="60" t="s">
+        <v>610</v>
+      </c>
+      <c r="B4" s="60" t="s">
+        <v>611</v>
+      </c>
+      <c r="C4" s="61" t="s">
+        <v>612</v>
+      </c>
+      <c r="D4" s="58"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
-        <v>609</v>
-      </c>
-      <c r="B5" s="68" t="s">
-        <v>344</v>
-      </c>
-      <c r="C5" s="68" t="s">
-        <v>610</v>
-      </c>
-      <c r="D5" s="67"/>
+      <c r="A5" s="60" t="s">
+        <v>613</v>
+      </c>
+      <c r="B5" s="60" t="s">
+        <v>470</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>614</v>
+      </c>
+      <c r="D5" s="58"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="69" t="s">
-        <v>611</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>408</v>
-      </c>
-      <c r="C6" s="70" t="s">
-        <v>612</v>
-      </c>
-      <c r="D6" s="67"/>
+      <c r="A6" s="65" t="s">
+        <v>615</v>
+      </c>
+      <c r="B6" s="65" t="s">
+        <v>616</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>617</v>
+      </c>
+      <c r="D6" s="58"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="71" t="s">
-        <v>613</v>
-      </c>
-      <c r="B7" s="72" t="s">
-        <v>403</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>614</v>
-      </c>
-      <c r="D7" s="67"/>
+      <c r="A7" s="65" t="s">
+        <v>618</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>402</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>619</v>
+      </c>
+      <c r="D7" s="58"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="69" t="s">
-        <v>615</v>
-      </c>
-      <c r="B8" s="69" t="s">
-        <v>616</v>
-      </c>
-      <c r="C8" s="70" t="s">
-        <v>617</v>
-      </c>
-      <c r="D8" s="67"/>
+      <c r="A8" s="65" t="s">
+        <v>620</v>
+      </c>
+      <c r="B8" s="65" t="s">
+        <v>402</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>621</v>
+      </c>
+      <c r="D8" s="58"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="69" t="s">
-        <v>618</v>
-      </c>
-      <c r="B9" s="69" t="s">
-        <v>471</v>
-      </c>
-      <c r="C9" s="70" t="s">
-        <v>619</v>
-      </c>
-      <c r="D9" s="67"/>
+      <c r="A9" s="60" t="s">
+        <v>543</v>
+      </c>
+      <c r="B9" s="60" t="s">
+        <v>447</v>
+      </c>
+      <c r="C9" s="61" t="s">
+        <v>622</v>
+      </c>
+      <c r="D9" s="58"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="74" t="s">
-        <v>620</v>
-      </c>
-      <c r="B10" s="74" t="s">
-        <v>621</v>
-      </c>
-      <c r="C10" s="73" t="s">
-        <v>622</v>
-      </c>
-      <c r="D10" s="67"/>
+      <c r="A10" s="60" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>623</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="74" t="s">
-        <v>623</v>
-      </c>
-      <c r="B11" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="C11" s="73" t="s">
+      <c r="A11" s="65" t="s">
+        <v>558</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>402</v>
+      </c>
+      <c r="C11" s="64" t="s">
         <v>624</v>
       </c>
-      <c r="D11" s="67"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="60" t="s">
         <v>625</v>
       </c>
-      <c r="B12" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="C12" s="73" t="s">
+      <c r="B12" s="60" t="s">
         <v>626</v>
       </c>
-      <c r="D12" s="67"/>
+      <c r="C12" s="61" t="s">
+        <v>627</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="69" t="s">
-        <v>544</v>
-      </c>
-      <c r="B13" s="69" t="s">
-        <v>448</v>
-      </c>
-      <c r="C13" s="70" t="s">
-        <v>627</v>
-      </c>
-      <c r="D13" s="67"/>
+      <c r="A13" s="60" t="s">
+        <v>628</v>
+      </c>
+      <c r="B13" s="60" t="s">
+        <v>629</v>
+      </c>
+      <c r="C13" s="61" t="s">
+        <v>630</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="69" t="s">
-        <v>550</v>
-      </c>
-      <c r="B14" s="69" t="s">
-        <v>403</v>
-      </c>
-      <c r="C14" s="70" t="s">
-        <v>628</v>
+      <c r="A14" s="65" t="s">
+        <v>631</v>
+      </c>
+      <c r="B14" s="65" t="s">
+        <v>402</v>
+      </c>
+      <c r="C14" s="64" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="74" t="s">
-        <v>559</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>403</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>629</v>
+      <c r="A15" s="60" t="s">
+        <v>633</v>
+      </c>
+      <c r="B15" s="60" t="s">
+        <v>634</v>
+      </c>
+      <c r="C15" s="61" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="69" t="s">
-        <v>630</v>
-      </c>
-      <c r="B16" s="69" t="s">
-        <v>631</v>
-      </c>
-      <c r="C16" s="70" t="s">
-        <v>632</v>
+      <c r="A16" s="60" t="s">
+        <v>636</v>
+      </c>
+      <c r="B16" s="60" t="s">
+        <v>402</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="69" t="s">
-        <v>633</v>
-      </c>
-      <c r="B17" s="69" t="s">
-        <v>634</v>
-      </c>
-      <c r="C17" s="70" t="s">
-        <v>635</v>
+      <c r="A17" s="65" t="s">
+        <v>636</v>
+      </c>
+      <c r="B17" s="65" t="s">
+        <v>402</v>
+      </c>
+      <c r="C17" s="64" t="s">
+        <v>638</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="74" t="s">
-        <v>636</v>
-      </c>
-      <c r="B18" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="C18" s="73" t="s">
-        <v>637</v>
+      <c r="A18" s="60" t="s">
+        <v>639</v>
+      </c>
+      <c r="B18" s="60" t="s">
+        <v>383</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="69" t="s">
-        <v>638</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>639</v>
-      </c>
-      <c r="C19" s="70" t="s">
-        <v>640</v>
+      <c r="A19" s="62" t="s">
+        <v>641</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>441</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="69" t="s">
-        <v>641</v>
-      </c>
-      <c r="B20" s="69" t="s">
-        <v>403</v>
-      </c>
-      <c r="C20" s="70" t="s">
-        <v>642</v>
+      <c r="A20" s="62" t="s">
+        <v>587</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>643</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="74" t="s">
-        <v>641</v>
-      </c>
-      <c r="B21" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="C21" s="73" t="s">
-        <v>643</v>
+      <c r="A21" s="62" t="s">
+        <v>590</v>
+      </c>
+      <c r="B21" s="62" t="s">
+        <v>402</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="69" t="s">
+      <c r="A22" s="65" t="s">
         <v>644</v>
       </c>
-      <c r="B22" s="69" t="s">
-        <v>384</v>
-      </c>
-      <c r="C22" s="70" t="s">
+      <c r="B22" s="65" t="s">
+        <v>402</v>
+      </c>
+      <c r="C22" s="64" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="71" t="s">
-        <v>646</v>
-      </c>
-      <c r="B23" s="72" t="s">
-        <v>442</v>
-      </c>
-      <c r="C23" s="75" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="71" t="s">
-        <v>588</v>
-      </c>
-      <c r="B24" s="71" t="s">
-        <v>648</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="71" t="s">
-        <v>591</v>
-      </c>
-      <c r="B25" s="71" t="s">
-        <v>403</v>
-      </c>
-      <c r="C25" s="75" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="74" t="s">
-        <v>649</v>
-      </c>
-      <c r="B26" s="74" t="s">
-        <v>403</v>
-      </c>
-      <c r="C26" s="73" t="s">
-        <v>650</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="C11" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="C12" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="C13" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="C14" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="C15" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="C16" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="C17" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
-    <hyperlink ref="C18" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="C19" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="C20" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
-    <hyperlink ref="C21" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
-    <hyperlink ref="C22" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
-    <hyperlink ref="C23" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
-    <hyperlink ref="C24" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
-    <hyperlink ref="C25" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
-    <hyperlink ref="C26" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="C5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="C6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="C7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="C8" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="C9" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="C11" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="C12" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="C13" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="C22" r:id="rId21" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10284,285 +10162,269 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="30.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
-    <col min="3" max="3" width="49.42578125" customWidth="1"/>
-    <col min="4" max="4" width="41.5703125" customWidth="1"/>
-    <col min="5" max="5" width="33" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="78" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B1" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="67" t="s">
+        <v>650</v>
+      </c>
+      <c r="B2" s="68" t="s">
         <v>651</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="69" t="s">
         <v>652</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="67" t="s">
         <v>653</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="E2" s="67" t="s">
         <v>654</v>
       </c>
+      <c r="F2" s="68" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="67" t="s">
+        <v>656</v>
+      </c>
+      <c r="B3" s="68"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
+    </row>
+    <row r="4" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
+        <v>657</v>
+      </c>
+      <c r="B4" s="68" t="s">
+        <v>658</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>659</v>
+      </c>
+      <c r="D4" s="67" t="s">
+        <v>660</v>
+      </c>
+      <c r="E4" s="67" t="s">
+        <v>661</v>
+      </c>
+      <c r="F4" s="68" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="67" t="s">
+        <v>663</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>664</v>
+      </c>
+      <c r="C5" s="71" t="s">
+        <v>665</v>
+      </c>
+      <c r="D5" s="67" t="s">
+        <v>666</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>667</v>
+      </c>
+      <c r="F5" s="68" t="s">
         <v>655</v>
       </c>
-      <c r="B3" s="77" t="s">
-        <v>656</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>657</v>
-      </c>
-      <c r="D3" s="76" t="s">
-        <v>658</v>
-      </c>
-      <c r="E3" s="76" t="s">
-        <v>659</v>
-      </c>
-      <c r="F3" s="77" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="76" t="s">
-        <v>661</v>
-      </c>
-      <c r="B4" s="77"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="77"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="76" t="s">
-        <v>662</v>
-      </c>
-      <c r="B5" s="77" t="s">
-        <v>663</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>664</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>665</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>666</v>
-      </c>
-      <c r="F5" s="77" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="76" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="67" t="s">
         <v>668</v>
       </c>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="68" t="s">
         <v>669</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="C6" s="70" t="s">
         <v>670</v>
       </c>
-      <c r="D6" s="76" t="s">
+      <c r="D6" s="67" t="s">
         <v>671</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="67" t="s">
         <v>672</v>
       </c>
-      <c r="F6" s="77" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="76" t="s">
+      <c r="F6" s="68" t="s">
         <v>673</v>
       </c>
-      <c r="B7" s="77" t="s">
+    </row>
+    <row r="7" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="67" t="s">
         <v>674</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="B7" s="68" t="s">
         <v>675</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="C7" s="70" t="s">
         <v>676</v>
       </c>
-      <c r="E7" s="76" t="s">
+      <c r="D7" s="67" t="s">
         <v>677</v>
       </c>
-      <c r="F7" s="77" t="s">
+      <c r="E7" s="67" t="s">
         <v>678</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="76" t="s">
+      <c r="F7" s="68" t="s">
         <v>679</v>
       </c>
-      <c r="B8" s="77" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="67" t="s">
         <v>680</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="B8" s="68" t="s">
         <v>681</v>
       </c>
-      <c r="D8" s="76" t="s">
+      <c r="C8" s="70" t="s">
         <v>682</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="D8" s="67" t="s">
         <v>683</v>
       </c>
-      <c r="F8" s="77" t="s">
+      <c r="E8" s="67" t="s">
         <v>684</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="s">
+      <c r="F8" s="68" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="67" t="s">
         <v>685</v>
       </c>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="68" t="s">
         <v>686</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="70" t="s">
         <v>687</v>
       </c>
-      <c r="D9" s="76" t="s">
+      <c r="D9" s="67" t="s">
         <v>688</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="67" t="s">
         <v>689</v>
       </c>
-      <c r="F9" s="77" t="s">
-        <v>660</v>
+      <c r="F9" s="68" t="s">
+        <v>690</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="76" t="s">
-        <v>690</v>
-      </c>
-      <c r="B10" s="77" t="s">
+      <c r="A10" s="67" t="s">
         <v>691</v>
       </c>
-      <c r="C10" s="79" t="s">
+      <c r="B10" s="68" t="s">
         <v>692</v>
       </c>
-      <c r="D10" s="76" t="s">
+      <c r="C10" s="70" t="s">
         <v>693</v>
       </c>
-      <c r="E10" s="76" t="s">
+      <c r="D10" s="67" t="s">
         <v>694</v>
       </c>
-      <c r="F10" s="77" t="s">
+      <c r="E10" s="67" t="s">
         <v>695</v>
       </c>
+      <c r="F10" s="68" t="s">
+        <v>655</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="67" t="s">
         <v>696</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="68"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+    </row>
+    <row r="12" spans="1:6" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="67" t="s">
         <v>697</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="B12" s="68" t="s">
         <v>698</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="C12" s="70" t="s">
         <v>699</v>
       </c>
-      <c r="E11" s="76" t="s">
+      <c r="D12" s="67" t="s">
         <v>700</v>
       </c>
-      <c r="F11" s="77" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="76" t="s">
+      <c r="E12" s="67" t="s">
         <v>701</v>
       </c>
-      <c r="B12" s="77"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="76" t="s">
+      <c r="F12" s="68" t="s">
         <v>702</v>
       </c>
-      <c r="B13" s="77" t="s">
+    </row>
+    <row r="13" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="67" t="s">
         <v>703</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="B13" s="68" t="s">
         <v>704</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="C13" s="70" t="s">
+        <v>320</v>
+      </c>
+      <c r="D13" s="67" t="s">
         <v>705</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="67" t="s">
         <v>706</v>
       </c>
-      <c r="F13" s="77" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="76" t="s">
-        <v>708</v>
-      </c>
-      <c r="B14" s="77" t="s">
-        <v>709</v>
-      </c>
-      <c r="C14" s="79" t="s">
-        <v>320</v>
-      </c>
-      <c r="D14" s="76" t="s">
-        <v>710</v>
-      </c>
-      <c r="E14" s="76" t="s">
-        <v>711</v>
-      </c>
-      <c r="F14" s="77" t="s">
-        <v>660</v>
+      <c r="F13" s="68" t="s">
+        <v>655</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="C5" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="C7" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="C9" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="C10" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="C11" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="C13" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="C14" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="C10" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="C13" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>